<commit_message>
Updated schemas for Varddokumentation and Konsultationsremiss according to service contract descritpion. Added greening information
</commit_message>
<xml_diff>
--- a/ServiceInteractions/riv/ehr/patientsummary/branches/TD_PATIENTSUMMARY_2/schemas/core_components/hl7cda/docs/CDA meddelandestruktur Varddokument v1 19.xlsx
+++ b/ServiceInteractions/riv/ehr/patientsummary/branches/TD_PATIENTSUMMARY_2/schemas/core_components/hl7cda/docs/CDA meddelandestruktur Varddokument v1 19.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22810"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="1995" windowWidth="11385" windowHeight="5430"/>
+    <workbookView xWindow="3980" yWindow="2000" windowWidth="18660" windowHeight="9220"/>
   </bookViews>
   <sheets>
     <sheet name="SendReferralAnswer CDA" sheetId="10" r:id="rId1"/>
     <sheet name="Instruktion för greening" sheetId="11" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -778,7 +783,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -825,6 +830,18 @@
       <color rgb="FFC00000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="8">
@@ -882,15 +899,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1085,6 +1104,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1094,16 +1121,10 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1403,42 +1424,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Blad2">
+  <sheetPr codeName="Blad2" enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:AR166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE101" sqref="AE101"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AE112" sqref="AE112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
-    <col min="2" max="5" width="2.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.6640625" style="1" customWidth="1"/>
+    <col min="2" max="5" width="2.5" style="1" customWidth="1"/>
     <col min="6" max="8" width="3" style="1" customWidth="1"/>
-    <col min="9" max="12" width="3.42578125" style="1" customWidth="1"/>
-    <col min="13" max="17" width="3.28515625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="5.5703125" style="1" customWidth="1"/>
+    <col min="9" max="12" width="3.5" style="1" customWidth="1"/>
+    <col min="13" max="17" width="3.33203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="5.5" style="1" customWidth="1"/>
     <col min="19" max="19" width="9" style="1" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="64.85546875" style="37" customWidth="1"/>
-    <col min="22" max="22" width="7.42578125" style="37" customWidth="1"/>
+    <col min="20" max="20" width="6.5" style="1" customWidth="1"/>
+    <col min="21" max="21" width="64.83203125" style="37" customWidth="1"/>
+    <col min="22" max="22" width="7.5" style="37" customWidth="1"/>
     <col min="23" max="23" width="7" style="37" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="1"/>
-    <col min="25" max="25" width="12.28515625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="15.7109375" style="1" customWidth="1"/>
-    <col min="28" max="28" width="29.28515625" style="45" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.83203125" style="1"/>
+    <col min="25" max="25" width="12.33203125" style="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5" style="1" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="29.33203125" style="45" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="14" style="45" customWidth="1"/>
-    <col min="30" max="30" width="10.5703125" style="45" customWidth="1"/>
-    <col min="31" max="31" width="64.28515625" style="64" customWidth="1"/>
-    <col min="32" max="32" width="41.42578125" style="1" customWidth="1"/>
-    <col min="33" max="16384" width="8.85546875" style="1"/>
+    <col min="30" max="30" width="10.5" style="45" customWidth="1"/>
+    <col min="31" max="31" width="64.33203125" style="64" customWidth="1"/>
+    <col min="32" max="32" width="41.5" style="1" customWidth="1"/>
+    <col min="33" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="2" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:44" s="2" customFormat="1" ht="2.25" customHeight="1">
       <c r="A1" s="34"/>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -1477,7 +1498,7 @@
       <c r="AJ1" s="36"/>
       <c r="AR1" s="8"/>
     </row>
-    <row r="2" spans="1:44" ht="6.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:44" ht="6.75" customHeight="1">
       <c r="A2" s="35"/>
       <c r="B2" s="35"/>
       <c r="C2" s="35"/>
@@ -1499,8 +1520,8 @@
       <c r="S2" s="35"/>
       <c r="T2" s="35"/>
       <c r="U2" s="25"/>
-      <c r="V2" s="78"/>
-      <c r="W2" s="78"/>
+      <c r="V2" s="82"/>
+      <c r="W2" s="82"/>
       <c r="X2" s="43"/>
       <c r="Y2" s="43"/>
       <c r="Z2" s="43"/>
@@ -1523,49 +1544,49 @@
       <c r="AQ2" s="2"/>
       <c r="AR2" s="2"/>
     </row>
-    <row r="3" spans="1:44" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="76" t="s">
+    <row r="3" spans="1:44" ht="27" customHeight="1">
+      <c r="A3" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="76"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="76"/>
-      <c r="Q3" s="76"/>
-      <c r="R3" s="76"/>
-      <c r="S3" s="76"/>
-      <c r="T3" s="76"/>
-      <c r="U3" s="77"/>
-      <c r="V3" s="78"/>
-      <c r="W3" s="78"/>
-      <c r="X3" s="78" t="s">
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="80"/>
+      <c r="P3" s="80"/>
+      <c r="Q3" s="80"/>
+      <c r="R3" s="80"/>
+      <c r="S3" s="80"/>
+      <c r="T3" s="80"/>
+      <c r="U3" s="81"/>
+      <c r="V3" s="82"/>
+      <c r="W3" s="82"/>
+      <c r="X3" s="82" t="s">
         <v>143</v>
       </c>
-      <c r="Y3" s="78"/>
-      <c r="Z3" s="78"/>
-      <c r="AA3" s="78"/>
-      <c r="AB3" s="78"/>
-      <c r="AC3" s="78"/>
-      <c r="AD3" s="78"/>
-      <c r="AE3" s="78"/>
-      <c r="AF3" s="78"/>
-      <c r="AG3" s="78"/>
-      <c r="AH3" s="78"/>
+      <c r="Y3" s="82"/>
+      <c r="Z3" s="82"/>
+      <c r="AA3" s="82"/>
+      <c r="AB3" s="82"/>
+      <c r="AC3" s="82"/>
+      <c r="AD3" s="82"/>
+      <c r="AE3" s="82"/>
+      <c r="AF3" s="82"/>
+      <c r="AG3" s="82"/>
+      <c r="AH3" s="82"/>
       <c r="AI3" s="36"/>
       <c r="AJ3" s="37"/>
     </row>
-    <row r="4" spans="1:44" s="2" customFormat="1" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:44" s="2" customFormat="1" ht="1.5" customHeight="1">
       <c r="A4" s="29"/>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
@@ -1603,7 +1624,7 @@
       <c r="AI4" s="38"/>
       <c r="AJ4" s="36"/>
     </row>
-    <row r="5" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:44" ht="30" customHeight="1">
       <c r="A5" s="27" t="s">
         <v>0</v>
       </c>
@@ -1651,7 +1672,7 @@
       <c r="AG5" s="39"/>
       <c r="AH5" s="39"/>
     </row>
-    <row r="6" spans="1:44" s="2" customFormat="1" ht="1.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:44" s="2" customFormat="1" ht="1.5" customHeight="1">
       <c r="A6" s="21"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
@@ -1687,7 +1708,7 @@
       <c r="AG6" s="42"/>
       <c r="AH6" s="42"/>
     </row>
-    <row r="7" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:44" ht="12.75" customHeight="1">
       <c r="A7" s="68" t="s">
         <v>144</v>
       </c>
@@ -1714,7 +1735,7 @@
       <c r="V7" s="49"/>
       <c r="W7" s="49"/>
     </row>
-    <row r="8" spans="1:44" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:44" s="2" customFormat="1" ht="10.5" customHeight="1">
       <c r="A8" s="68" t="s">
         <v>52</v>
       </c>
@@ -1747,7 +1768,7 @@
       <c r="AD8" s="3"/>
       <c r="AE8" s="47"/>
     </row>
-    <row r="9" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:44" s="2" customFormat="1">
       <c r="A9" s="68" t="s">
         <v>144</v>
       </c>
@@ -1771,10 +1792,10 @@
       <c r="S9" s="49"/>
       <c r="T9" s="49"/>
       <c r="U9" s="6"/>
-      <c r="V9" s="79" t="s">
+      <c r="V9" s="76" t="s">
         <v>245</v>
       </c>
-      <c r="W9" s="80"/>
+      <c r="W9" s="77"/>
       <c r="AB9" s="48" t="s">
         <v>246</v>
       </c>
@@ -1782,7 +1803,7 @@
       <c r="AD9" s="3"/>
       <c r="AE9" s="47"/>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:44">
       <c r="A10" s="49" t="s">
         <v>6</v>
       </c>
@@ -1806,15 +1827,15 @@
       <c r="S10" s="49"/>
       <c r="T10" s="49"/>
       <c r="U10" s="7"/>
-      <c r="V10" s="81"/>
-      <c r="W10" s="82" t="s">
+      <c r="V10" s="78"/>
+      <c r="W10" s="79" t="s">
         <v>244</v>
       </c>
       <c r="AB10" s="17" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:44" s="2" customFormat="1">
       <c r="A11" s="49"/>
       <c r="B11" s="49" t="s">
         <v>7</v>
@@ -1851,7 +1872,7 @@
       <c r="AD11" s="3"/>
       <c r="AE11" s="47"/>
     </row>
-    <row r="12" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:44" s="2" customFormat="1">
       <c r="A12" s="49"/>
       <c r="B12" s="49"/>
       <c r="C12" s="49" t="s">
@@ -1893,7 +1914,7 @@
       <c r="AD12" s="3"/>
       <c r="AE12" s="47"/>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:44">
       <c r="A13" s="49"/>
       <c r="B13" s="49"/>
       <c r="C13" s="49" t="s">
@@ -1929,7 +1950,7 @@
       <c r="Z13" s="45"/>
       <c r="AA13" s="45"/>
     </row>
-    <row r="14" spans="1:44" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:44" s="2" customFormat="1">
       <c r="A14" s="49"/>
       <c r="B14" s="49" t="s">
         <v>8</v>
@@ -1977,7 +1998,7 @@
       </c>
       <c r="AF14" s="47"/>
     </row>
-    <row r="15" spans="1:44" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:44" s="2" customFormat="1">
       <c r="A15" s="49"/>
       <c r="B15" s="49"/>
       <c r="C15" s="49" t="s">
@@ -2018,7 +2039,7 @@
       <c r="AD15" s="3"/>
       <c r="AE15" s="47"/>
     </row>
-    <row r="16" spans="1:44" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:44" s="2" customFormat="1" ht="13.5" customHeight="1">
       <c r="A16" s="49"/>
       <c r="B16" s="49"/>
       <c r="C16" s="49" t="s">
@@ -2060,7 +2081,7 @@
       <c r="AD16" s="3"/>
       <c r="AE16" s="47"/>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32">
       <c r="A17" s="49"/>
       <c r="B17" s="49" t="s">
         <v>9</v>
@@ -2093,7 +2114,7 @@
       <c r="Z17" s="45"/>
       <c r="AA17" s="45"/>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32">
       <c r="A18" s="49"/>
       <c r="B18" s="49"/>
       <c r="C18" s="49" t="s">
@@ -2130,7 +2151,7 @@
       <c r="Z18" s="45"/>
       <c r="AA18" s="45"/>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32">
       <c r="A19" s="49"/>
       <c r="B19" s="49"/>
       <c r="C19" s="49" t="s">
@@ -2167,7 +2188,7 @@
       <c r="Z19" s="45"/>
       <c r="AA19" s="45"/>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32">
       <c r="A20" s="49"/>
       <c r="B20" s="49" t="s">
         <v>33</v>
@@ -2215,7 +2236,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="21" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:32" s="2" customFormat="1">
       <c r="A21" s="49"/>
       <c r="B21" s="49" t="s">
         <v>26</v>
@@ -2254,7 +2275,7 @@
       <c r="AD21" s="3"/>
       <c r="AE21" s="47"/>
     </row>
-    <row r="22" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32" s="2" customFormat="1">
       <c r="A22" s="15"/>
       <c r="B22" s="15"/>
       <c r="C22" s="15" t="s">
@@ -2305,7 +2326,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="23" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" s="2" customFormat="1">
       <c r="A23" s="15"/>
       <c r="B23" s="55" t="s">
         <v>35</v>
@@ -2342,7 +2363,7 @@
       <c r="AD23" s="3"/>
       <c r="AE23" s="47"/>
     </row>
-    <row r="24" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" s="2" customFormat="1">
       <c r="A24" s="15"/>
       <c r="B24" s="15"/>
       <c r="C24" s="55" t="s">
@@ -2384,7 +2405,7 @@
       <c r="AD24" s="3"/>
       <c r="AE24" s="47"/>
     </row>
-    <row r="25" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32" s="2" customFormat="1">
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
       <c r="C25" s="55" t="s">
@@ -2424,7 +2445,7 @@
       <c r="AD25" s="3"/>
       <c r="AE25" s="47"/>
     </row>
-    <row r="26" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:32" s="2" customFormat="1">
       <c r="A26" s="15"/>
       <c r="B26" s="55" t="s">
         <v>10</v>
@@ -2463,7 +2484,7 @@
       <c r="AD26" s="3"/>
       <c r="AE26" s="47"/>
     </row>
-    <row r="27" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:32" s="2" customFormat="1">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
       <c r="C27" s="55" t="s">
@@ -2500,7 +2521,7 @@
       <c r="AD27" s="3"/>
       <c r="AE27" s="3"/>
     </row>
-    <row r="28" spans="1:32" s="2" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:32" s="2" customFormat="1" ht="96">
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
       <c r="C28" s="55"/>
@@ -2548,7 +2569,7 @@
       </c>
       <c r="AF28" s="47"/>
     </row>
-    <row r="29" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:32" s="2" customFormat="1">
       <c r="A29" s="15"/>
       <c r="B29" s="55"/>
       <c r="C29" s="15"/>
@@ -2589,7 +2610,7 @@
       <c r="AD29" s="3"/>
       <c r="AE29" s="47"/>
     </row>
-    <row r="30" spans="1:32" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:32" s="2" customFormat="1" ht="36">
       <c r="A30" s="15"/>
       <c r="B30" s="15"/>
       <c r="C30" s="55"/>
@@ -2630,7 +2651,7 @@
       <c r="AD30" s="3"/>
       <c r="AE30" s="47"/>
     </row>
-    <row r="31" spans="1:32" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:32" s="2" customFormat="1" ht="24">
       <c r="A31" s="15"/>
       <c r="B31" s="15" t="s">
         <v>12</v>
@@ -2677,7 +2698,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="32" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:32" s="2" customFormat="1">
       <c r="A32" s="15"/>
       <c r="B32" s="15"/>
       <c r="C32" s="55" t="s">
@@ -2716,7 +2737,7 @@
       <c r="AD32" s="3"/>
       <c r="AE32" s="47"/>
     </row>
-    <row r="33" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:32" s="2" customFormat="1">
       <c r="A33" s="15"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -2767,7 +2788,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="34" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:32" s="2" customFormat="1">
       <c r="A34" s="15"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15" t="s">
@@ -2805,7 +2826,7 @@
       <c r="AE34" s="47"/>
       <c r="AF34" s="33"/>
     </row>
-    <row r="35" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A35" s="15"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
@@ -2844,7 +2865,7 @@
       <c r="AD35" s="3"/>
       <c r="AE35" s="47"/>
     </row>
-    <row r="36" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A36" s="15"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
@@ -2895,7 +2916,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="37" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A37" s="15"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -2937,7 +2958,7 @@
       <c r="AD37" s="3"/>
       <c r="AE37" s="47"/>
     </row>
-    <row r="38" spans="1:32" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:32" s="2" customFormat="1" ht="48">
       <c r="A38" s="15"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
@@ -2984,7 +3005,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="39" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A39" s="15"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
@@ -3025,7 +3046,7 @@
       <c r="AD39" s="3"/>
       <c r="AE39" s="47"/>
     </row>
-    <row r="40" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A40" s="15"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
@@ -3066,7 +3087,7 @@
       <c r="AD40" s="3"/>
       <c r="AE40" s="47"/>
     </row>
-    <row r="41" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A41" s="15"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
@@ -3107,7 +3128,7 @@
       <c r="AD41" s="3"/>
       <c r="AE41" s="47"/>
     </row>
-    <row r="42" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A42" s="15"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
@@ -3144,7 +3165,7 @@
       <c r="AD42" s="3"/>
       <c r="AE42" s="47"/>
     </row>
-    <row r="43" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A43" s="15"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
@@ -3193,7 +3214,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="44" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A44" s="15"/>
       <c r="B44" s="36"/>
       <c r="C44" s="15"/>
@@ -3230,7 +3251,7 @@
       <c r="AD44" s="3"/>
       <c r="AE44" s="47"/>
     </row>
-    <row r="45" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A45" s="15"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
@@ -3279,7 +3300,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -3320,7 +3341,7 @@
       <c r="AD46" s="3"/>
       <c r="AE46" s="47"/>
     </row>
-    <row r="47" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A47" s="15"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
@@ -3361,7 +3382,7 @@
       <c r="AD47" s="3"/>
       <c r="AE47" s="47"/>
     </row>
-    <row r="48" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:32" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A48" s="15"/>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -3411,7 +3432,7 @@
       </c>
       <c r="AF48" s="3"/>
     </row>
-    <row r="49" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A49" s="15"/>
       <c r="B49" s="15"/>
       <c r="C49" s="15"/>
@@ -3460,7 +3481,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="50" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A50" s="15"/>
       <c r="B50" s="15"/>
       <c r="C50" s="15"/>
@@ -3510,7 +3531,7 @@
       </c>
       <c r="AF50" s="3"/>
     </row>
-    <row r="51" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A51" s="15"/>
       <c r="B51" s="15"/>
       <c r="C51" s="15"/>
@@ -3549,7 +3570,7 @@
       <c r="AD51" s="3"/>
       <c r="AE51" s="47"/>
     </row>
-    <row r="52" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A52" s="15"/>
       <c r="B52" s="15"/>
       <c r="C52" s="15"/>
@@ -3586,7 +3607,7 @@
       <c r="AD52" s="3"/>
       <c r="AE52" s="47"/>
     </row>
-    <row r="53" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A53" s="15"/>
       <c r="B53" s="15"/>
       <c r="C53" s="15"/>
@@ -3625,7 +3646,7 @@
       <c r="AD53" s="3"/>
       <c r="AE53" s="47"/>
     </row>
-    <row r="54" spans="1:34" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:34" s="2" customFormat="1" ht="30" customHeight="1">
       <c r="A54" s="15"/>
       <c r="B54" s="15"/>
       <c r="C54" s="15"/>
@@ -3676,7 +3697,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="55" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:34" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A55" s="15"/>
       <c r="B55" s="15"/>
       <c r="C55" s="15"/>
@@ -3717,7 +3738,7 @@
       <c r="AD55" s="3"/>
       <c r="AE55" s="47"/>
     </row>
-    <row r="56" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:34" s="2" customFormat="1">
       <c r="A56" s="15"/>
       <c r="B56" s="15" t="s">
         <v>16</v>
@@ -3756,7 +3777,7 @@
       <c r="AD56" s="3"/>
       <c r="AE56" s="47"/>
     </row>
-    <row r="57" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:34" s="2" customFormat="1">
       <c r="A57" s="15"/>
       <c r="B57" s="15"/>
       <c r="C57" s="15" t="s">
@@ -3794,7 +3815,7 @@
       <c r="AE57" s="47"/>
       <c r="AF57" s="3"/>
     </row>
-    <row r="58" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:34" s="2" customFormat="1">
       <c r="A58" s="15"/>
       <c r="B58" s="15"/>
       <c r="C58" s="15"/>
@@ -3831,7 +3852,7 @@
       <c r="AD58" s="3"/>
       <c r="AE58" s="47"/>
     </row>
-    <row r="59" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:34" s="2" customFormat="1">
       <c r="A59" s="15"/>
       <c r="B59" s="15"/>
       <c r="C59" s="15"/>
@@ -3870,7 +3891,7 @@
       <c r="AD59" s="3"/>
       <c r="AE59" s="47"/>
     </row>
-    <row r="60" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:34" s="2" customFormat="1">
       <c r="A60" s="15"/>
       <c r="B60" s="15"/>
       <c r="C60" s="15"/>
@@ -3924,7 +3945,7 @@
       <c r="AG60" s="32"/>
       <c r="AH60" s="32"/>
     </row>
-    <row r="61" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:34" s="2" customFormat="1">
       <c r="A61" s="15"/>
       <c r="B61" s="15"/>
       <c r="C61" s="15"/>
@@ -3966,7 +3987,7 @@
       <c r="AD61" s="3"/>
       <c r="AE61" s="47"/>
     </row>
-    <row r="62" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:34" s="2" customFormat="1">
       <c r="A62" s="15"/>
       <c r="B62" s="15" t="s">
         <v>19</v>
@@ -4013,7 +4034,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="63" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:34" s="2" customFormat="1">
       <c r="A63" s="15"/>
       <c r="B63" s="15"/>
       <c r="C63" s="55" t="s">
@@ -4050,7 +4071,7 @@
       <c r="AD63" s="3"/>
       <c r="AE63" s="47"/>
     </row>
-    <row r="64" spans="1:34" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:34" s="2" customFormat="1" ht="24">
       <c r="A64" s="15"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
@@ -4101,7 +4122,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="65" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:31" s="2" customFormat="1">
       <c r="A65" s="15"/>
       <c r="B65" s="15"/>
       <c r="C65" s="55" t="s">
@@ -4138,7 +4159,7 @@
       <c r="AD65" s="3"/>
       <c r="AE65" s="47"/>
     </row>
-    <row r="66" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:31" s="2" customFormat="1">
       <c r="A66" s="15"/>
       <c r="B66" s="15"/>
       <c r="C66" s="15"/>
@@ -4178,7 +4199,7 @@
       <c r="AD66" s="3"/>
       <c r="AE66" s="3"/>
     </row>
-    <row r="67" spans="1:31" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:31" s="2" customFormat="1" ht="24">
       <c r="A67" s="15"/>
       <c r="B67" s="15"/>
       <c r="C67" s="15" t="s">
@@ -4225,7 +4246,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="68" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:31" s="2" customFormat="1">
       <c r="A68" s="15"/>
       <c r="B68" s="15"/>
       <c r="C68" s="15"/>
@@ -4264,7 +4285,7 @@
       <c r="AD68" s="3"/>
       <c r="AE68" s="3"/>
     </row>
-    <row r="69" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:31" s="2" customFormat="1">
       <c r="A69" s="15"/>
       <c r="B69" s="15"/>
       <c r="C69" s="15"/>
@@ -4315,7 +4336,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="70" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:31" s="2" customFormat="1">
       <c r="A70" s="15"/>
       <c r="B70" s="15"/>
       <c r="C70" s="15"/>
@@ -4357,7 +4378,7 @@
       <c r="AD70" s="3"/>
       <c r="AE70" s="47"/>
     </row>
-    <row r="71" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:31" s="2" customFormat="1">
       <c r="A71" s="15"/>
       <c r="B71" s="15"/>
       <c r="C71" s="15"/>
@@ -4394,7 +4415,7 @@
       <c r="AD71" s="3"/>
       <c r="AE71" s="47"/>
     </row>
-    <row r="72" spans="1:31" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:31" s="2" customFormat="1" ht="24">
       <c r="A72" s="15"/>
       <c r="B72" s="15"/>
       <c r="C72" s="15"/>
@@ -4433,7 +4454,7 @@
       <c r="AD72" s="3"/>
       <c r="AE72" s="47"/>
     </row>
-    <row r="73" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:31" s="2" customFormat="1">
       <c r="A73" s="15"/>
       <c r="B73" s="15"/>
       <c r="C73" s="15"/>
@@ -4484,7 +4505,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="74" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:31" s="2" customFormat="1">
       <c r="A74" s="15"/>
       <c r="B74" s="15"/>
       <c r="C74" s="15"/>
@@ -4525,7 +4546,7 @@
       <c r="AD74" s="3"/>
       <c r="AE74" s="47"/>
     </row>
-    <row r="75" spans="1:31" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:31" s="2" customFormat="1" ht="24">
       <c r="A75" s="15"/>
       <c r="B75" s="56" t="s">
         <v>57</v>
@@ -4572,7 +4593,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="76" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:31" s="2" customFormat="1">
       <c r="A76" s="15"/>
       <c r="B76" s="36"/>
       <c r="C76" s="15" t="s">
@@ -4609,7 +4630,7 @@
       <c r="AD76" s="3"/>
       <c r="AE76" s="47"/>
     </row>
-    <row r="77" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:31" s="2" customFormat="1">
       <c r="A77" s="15"/>
       <c r="B77" s="36"/>
       <c r="C77" s="15"/>
@@ -4648,7 +4669,7 @@
       <c r="AD77" s="3"/>
       <c r="AE77" s="47"/>
     </row>
-    <row r="78" spans="1:31" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:31" s="2" customFormat="1" ht="24">
       <c r="A78" s="15"/>
       <c r="B78" s="36"/>
       <c r="C78" s="15"/>
@@ -4689,7 +4710,7 @@
       <c r="AD78" s="3"/>
       <c r="AE78" s="47"/>
     </row>
-    <row r="79" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:31" s="2" customFormat="1">
       <c r="A79" s="15"/>
       <c r="B79" s="36"/>
       <c r="C79" s="15"/>
@@ -4730,7 +4751,7 @@
       <c r="AD79" s="3"/>
       <c r="AE79" s="47"/>
     </row>
-    <row r="80" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:31" s="2" customFormat="1">
       <c r="A80" s="15"/>
       <c r="B80" s="36"/>
       <c r="C80" s="15"/>
@@ -4767,7 +4788,7 @@
       <c r="AD80" s="3"/>
       <c r="AE80" s="47"/>
     </row>
-    <row r="81" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:31" s="2" customFormat="1">
       <c r="A81" s="15"/>
       <c r="B81" s="36"/>
       <c r="C81" s="15"/>
@@ -4806,7 +4827,7 @@
       <c r="AD81" s="3"/>
       <c r="AE81" s="47"/>
     </row>
-    <row r="82" spans="1:31" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:31" s="2" customFormat="1" ht="24">
       <c r="A82" s="15"/>
       <c r="B82" s="56" t="s">
         <v>60</v>
@@ -4845,7 +4866,7 @@
       <c r="AD82" s="3"/>
       <c r="AE82" s="47"/>
     </row>
-    <row r="83" spans="1:31" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:31" s="2" customFormat="1" ht="24">
       <c r="A83" s="15"/>
       <c r="B83" s="36"/>
       <c r="C83" s="55" t="s">
@@ -4890,7 +4911,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="84" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:31" s="2" customFormat="1">
       <c r="A84" s="15"/>
       <c r="B84" s="36"/>
       <c r="C84" s="15"/>
@@ -4937,7 +4958,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="85" spans="1:31" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:31" s="2" customFormat="1" ht="24">
       <c r="A85" s="15"/>
       <c r="B85" s="36"/>
       <c r="C85" s="15"/>
@@ -4978,7 +4999,7 @@
       <c r="AD85" s="3"/>
       <c r="AE85" s="47"/>
     </row>
-    <row r="86" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:31" s="2" customFormat="1">
       <c r="A86" s="15"/>
       <c r="B86" s="36"/>
       <c r="C86" s="15"/>
@@ -5017,7 +5038,7 @@
       <c r="AD86" s="3"/>
       <c r="AE86" s="47"/>
     </row>
-    <row r="87" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:31" s="2" customFormat="1">
       <c r="A87" s="15"/>
       <c r="B87" s="36"/>
       <c r="C87" s="15"/>
@@ -5066,7 +5087,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="88" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:31" s="2" customFormat="1">
       <c r="A88" s="15"/>
       <c r="B88" s="36"/>
       <c r="C88" s="15"/>
@@ -5117,7 +5138,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="89" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:31" s="2" customFormat="1">
       <c r="A89" s="15"/>
       <c r="B89" s="36"/>
       <c r="C89" s="15"/>
@@ -5160,7 +5181,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="90" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:31" s="2" customFormat="1">
       <c r="A90" s="15"/>
       <c r="B90" s="36"/>
       <c r="C90" s="15"/>
@@ -5193,7 +5214,7 @@
       <c r="AD90" s="3"/>
       <c r="AE90" s="47"/>
     </row>
-    <row r="91" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:31" s="2" customFormat="1">
       <c r="A91" s="36"/>
       <c r="B91" s="71" t="s">
         <v>5</v>
@@ -5228,7 +5249,7 @@
       <c r="AD91" s="3"/>
       <c r="AE91" s="47"/>
     </row>
-    <row r="92" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:31" s="2" customFormat="1">
       <c r="A92" s="36"/>
       <c r="B92" s="71" t="s">
         <v>21</v>
@@ -5267,7 +5288,7 @@
       <c r="AD92" s="3"/>
       <c r="AE92" s="47"/>
     </row>
-    <row r="93" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:31" s="2" customFormat="1">
       <c r="A93" s="36"/>
       <c r="B93" s="71" t="s">
         <v>5</v>
@@ -5302,7 +5323,7 @@
       <c r="AD93" s="3"/>
       <c r="AE93" s="47"/>
     </row>
-    <row r="94" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:31" s="2" customFormat="1">
       <c r="A94" s="15"/>
       <c r="B94" s="15" t="s">
         <v>22</v>
@@ -5339,7 +5360,7 @@
       <c r="AD94" s="3"/>
       <c r="AE94" s="47"/>
     </row>
-    <row r="95" spans="1:31" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:31" s="4" customFormat="1">
       <c r="A95" s="15"/>
       <c r="B95" s="15"/>
       <c r="C95" s="15" t="s">
@@ -5376,7 +5397,7 @@
       <c r="AD95" s="5"/>
       <c r="AE95" s="65"/>
     </row>
-    <row r="96" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:31" s="2" customFormat="1">
       <c r="A96" s="36"/>
       <c r="B96" s="71" t="s">
         <v>5</v>
@@ -5411,7 +5432,7 @@
       <c r="AD96" s="3"/>
       <c r="AE96" s="47"/>
     </row>
-    <row r="97" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:32" s="2" customFormat="1">
       <c r="A97" s="36"/>
       <c r="B97" s="71" t="s">
         <v>63</v>
@@ -5446,7 +5467,7 @@
       <c r="AD97" s="3"/>
       <c r="AE97" s="47"/>
     </row>
-    <row r="98" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:32" s="2" customFormat="1">
       <c r="A98" s="36"/>
       <c r="B98" s="71" t="s">
         <v>5</v>
@@ -5481,7 +5502,7 @@
       <c r="AD98" s="3"/>
       <c r="AE98" s="47"/>
     </row>
-    <row r="99" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:32" s="2" customFormat="1">
       <c r="A99" s="15"/>
       <c r="B99" s="15"/>
       <c r="C99" s="15"/>
@@ -5528,7 +5549,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="100" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:32" s="2" customFormat="1">
       <c r="A100" s="15"/>
       <c r="B100" s="15"/>
       <c r="C100" s="15"/>
@@ -5565,7 +5586,7 @@
       <c r="AD100" s="3"/>
       <c r="AE100" s="47"/>
     </row>
-    <row r="101" spans="1:32" s="2" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:32" s="2" customFormat="1" ht="105.75" customHeight="1">
       <c r="A101" s="15"/>
       <c r="B101" s="15"/>
       <c r="C101" s="15"/>
@@ -5614,7 +5635,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="102" spans="1:32" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:32" s="2" customFormat="1" ht="60">
       <c r="A102" s="15"/>
       <c r="B102" s="15"/>
       <c r="C102" s="15"/>
@@ -5655,7 +5676,7 @@
       <c r="AD102" s="3"/>
       <c r="AE102" s="47"/>
     </row>
-    <row r="103" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:32" s="2" customFormat="1">
       <c r="A103" s="15"/>
       <c r="B103" s="15"/>
       <c r="C103" s="15"/>
@@ -5696,7 +5717,7 @@
       <c r="AD103" s="3"/>
       <c r="AE103" s="47"/>
     </row>
-    <row r="104" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:32" s="2" customFormat="1">
       <c r="A104" s="15"/>
       <c r="B104" s="15"/>
       <c r="C104" s="15"/>
@@ -5745,7 +5766,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="105" spans="1:32" s="2" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:32" s="2" customFormat="1" ht="72">
       <c r="A105" s="15"/>
       <c r="B105" s="15"/>
       <c r="C105" s="15"/>
@@ -5795,7 +5816,7 @@
       </c>
       <c r="AF105" s="12"/>
     </row>
-    <row r="106" spans="1:32" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:32" s="2" customFormat="1" ht="24">
       <c r="A106" s="15"/>
       <c r="B106" s="15"/>
       <c r="C106" s="15"/>
@@ -5835,7 +5856,7 @@
       <c r="AE106" s="47"/>
       <c r="AF106" s="12"/>
     </row>
-    <row r="107" spans="1:32" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:32" s="2" customFormat="1" ht="36">
       <c r="A107" s="15"/>
       <c r="B107" s="15"/>
       <c r="C107" s="15"/>
@@ -5876,7 +5897,7 @@
       <c r="AD107" s="3"/>
       <c r="AE107" s="47"/>
     </row>
-    <row r="108" spans="1:32" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:32" s="2" customFormat="1" ht="36">
       <c r="A108" s="15"/>
       <c r="B108" s="15"/>
       <c r="C108" s="15"/>
@@ -5923,7 +5944,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="109" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:32" s="2" customFormat="1">
       <c r="A109" s="15"/>
       <c r="B109" s="15"/>
       <c r="C109" s="15"/>
@@ -5960,7 +5981,7 @@
       <c r="AD109" s="3"/>
       <c r="AE109" s="47"/>
     </row>
-    <row r="110" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:32" s="2" customFormat="1">
       <c r="A110" s="15"/>
       <c r="B110" s="15"/>
       <c r="C110" s="15"/>
@@ -5999,7 +6020,7 @@
       <c r="AD110" s="3"/>
       <c r="AE110" s="47"/>
     </row>
-    <row r="111" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:32" s="2" customFormat="1">
       <c r="A111" s="15"/>
       <c r="B111" s="15"/>
       <c r="C111" s="15"/>
@@ -6038,7 +6059,7 @@
       <c r="AD111" s="3"/>
       <c r="AE111" s="47"/>
     </row>
-    <row r="112" spans="1:32" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:32" s="2" customFormat="1" ht="36">
       <c r="A112" s="15"/>
       <c r="B112" s="15"/>
       <c r="C112" s="15"/>
@@ -6087,7 +6108,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="113" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:31" s="2" customFormat="1">
       <c r="A113" s="15"/>
       <c r="B113" s="15"/>
       <c r="C113" s="15"/>
@@ -6136,7 +6157,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="114" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:31" s="2" customFormat="1">
       <c r="A114" s="15"/>
       <c r="B114" s="15"/>
       <c r="C114" s="15"/>
@@ -6185,7 +6206,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="115" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:31" s="2" customFormat="1">
       <c r="A115" s="15"/>
       <c r="B115" s="15"/>
       <c r="C115" s="15"/>
@@ -6234,7 +6255,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="116" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:31" s="2" customFormat="1">
       <c r="A116" s="15"/>
       <c r="B116" s="15"/>
       <c r="C116" s="15"/>
@@ -6275,7 +6296,7 @@
       <c r="AD116" s="3"/>
       <c r="AE116" s="47"/>
     </row>
-    <row r="117" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:31" s="2" customFormat="1">
       <c r="A117" s="15"/>
       <c r="B117" s="15"/>
       <c r="C117" s="15"/>
@@ -6314,7 +6335,7 @@
       <c r="AD117" s="3"/>
       <c r="AE117" s="47"/>
     </row>
-    <row r="118" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:31" s="2" customFormat="1">
       <c r="A118" s="15"/>
       <c r="B118" s="15" t="s">
         <v>5</v>
@@ -6349,7 +6370,7 @@
       <c r="AD118" s="3"/>
       <c r="AE118" s="47"/>
     </row>
-    <row r="119" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:31" s="2" customFormat="1">
       <c r="A119" s="15"/>
       <c r="B119" s="15"/>
       <c r="C119" s="15"/>
@@ -6382,7 +6403,7 @@
       <c r="AD119" s="3"/>
       <c r="AE119" s="47"/>
     </row>
-    <row r="120" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:31" s="2" customFormat="1">
       <c r="A120" s="4"/>
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
@@ -6415,7 +6436,7 @@
       <c r="AD120" s="3"/>
       <c r="AE120" s="47"/>
     </row>
-    <row r="121" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:31" s="2" customFormat="1">
       <c r="A121" s="4"/>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
@@ -6444,7 +6465,7 @@
       <c r="AD121" s="3"/>
       <c r="AE121" s="47"/>
     </row>
-    <row r="122" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:31" s="2" customFormat="1">
       <c r="A122" s="4"/>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
@@ -6471,7 +6492,7 @@
       <c r="AD122" s="3"/>
       <c r="AE122" s="47"/>
     </row>
-    <row r="123" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:31" s="2" customFormat="1">
       <c r="A123" s="4"/>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
@@ -6498,7 +6519,7 @@
       <c r="AD123" s="3"/>
       <c r="AE123" s="47"/>
     </row>
-    <row r="124" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:31" s="2" customFormat="1">
       <c r="A124" s="4"/>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
@@ -6525,7 +6546,7 @@
       <c r="AD124" s="3"/>
       <c r="AE124" s="47"/>
     </row>
-    <row r="125" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:31" s="2" customFormat="1">
       <c r="A125" s="4"/>
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
@@ -6549,7 +6570,7 @@
       <c r="AD125" s="3"/>
       <c r="AE125" s="47"/>
     </row>
-    <row r="126" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:31" s="2" customFormat="1">
       <c r="A126" s="4"/>
       <c r="E126" s="4"/>
       <c r="F126" s="4"/>
@@ -6572,7 +6593,7 @@
       <c r="AD126" s="3"/>
       <c r="AE126" s="47"/>
     </row>
-    <row r="127" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:31" s="2" customFormat="1">
       <c r="A127" s="4"/>
       <c r="E127" s="4"/>
       <c r="F127" s="4"/>
@@ -6596,7 +6617,7 @@
       <c r="AD127" s="3"/>
       <c r="AE127" s="47"/>
     </row>
-    <row r="128" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:31" s="2" customFormat="1">
       <c r="A128" s="4"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
@@ -6621,7 +6642,7 @@
       <c r="AD128" s="3"/>
       <c r="AE128" s="47"/>
     </row>
-    <row r="129" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:31" s="2" customFormat="1">
       <c r="A129" s="4"/>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
@@ -6646,7 +6667,7 @@
       <c r="AD129" s="3"/>
       <c r="AE129" s="47"/>
     </row>
-    <row r="130" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:31" s="2" customFormat="1">
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
@@ -6670,7 +6691,7 @@
       <c r="AD130" s="3"/>
       <c r="AE130" s="47"/>
     </row>
-    <row r="131" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:31" s="2" customFormat="1">
       <c r="A131" s="4"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
@@ -6694,7 +6715,7 @@
       <c r="AD131" s="3"/>
       <c r="AE131" s="47"/>
     </row>
-    <row r="132" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:31" s="2" customFormat="1">
       <c r="A132" s="4"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
@@ -6719,7 +6740,7 @@
       <c r="AD132" s="3"/>
       <c r="AE132" s="47"/>
     </row>
-    <row r="133" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:31" s="2" customFormat="1">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
@@ -6746,7 +6767,7 @@
       <c r="AD133" s="3"/>
       <c r="AE133" s="47"/>
     </row>
-    <row r="134" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:31" s="2" customFormat="1">
       <c r="A134" s="4"/>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
@@ -6775,7 +6796,7 @@
       <c r="AD134" s="3"/>
       <c r="AE134" s="47"/>
     </row>
-    <row r="135" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:31" s="2" customFormat="1">
       <c r="A135" s="4"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
@@ -6804,7 +6825,7 @@
       <c r="AD135" s="3"/>
       <c r="AE135" s="47"/>
     </row>
-    <row r="136" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:31" s="2" customFormat="1">
       <c r="A136" s="4"/>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
@@ -6833,7 +6854,7 @@
       <c r="AD136" s="3"/>
       <c r="AE136" s="47"/>
     </row>
-    <row r="137" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:31" s="2" customFormat="1">
       <c r="A137" s="4"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
@@ -6862,7 +6883,7 @@
       <c r="AD137" s="3"/>
       <c r="AE137" s="47"/>
     </row>
-    <row r="138" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:31" s="2" customFormat="1">
       <c r="A138" s="4"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
@@ -6889,7 +6910,7 @@
       <c r="AD138" s="3"/>
       <c r="AE138" s="47"/>
     </row>
-    <row r="139" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:31" s="2" customFormat="1">
       <c r="A139" s="4"/>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
@@ -6916,7 +6937,7 @@
       <c r="AD139" s="3"/>
       <c r="AE139" s="47"/>
     </row>
-    <row r="140" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:31" s="2" customFormat="1">
       <c r="A140" s="4"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
@@ -6943,7 +6964,7 @@
       <c r="AD140" s="3"/>
       <c r="AE140" s="47"/>
     </row>
-    <row r="141" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:31" s="2" customFormat="1">
       <c r="A141" s="4"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
@@ -6970,7 +6991,7 @@
       <c r="AD141" s="3"/>
       <c r="AE141" s="47"/>
     </row>
-    <row r="142" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:31" s="2" customFormat="1">
       <c r="A142" s="4"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
@@ -6997,7 +7018,7 @@
       <c r="AD142" s="3"/>
       <c r="AE142" s="47"/>
     </row>
-    <row r="143" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:31" s="2" customFormat="1">
       <c r="A143" s="4"/>
       <c r="B143" s="4"/>
       <c r="C143" s="4"/>
@@ -7024,7 +7045,7 @@
       <c r="AD143" s="3"/>
       <c r="AE143" s="47"/>
     </row>
-    <row r="144" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:31" s="2" customFormat="1">
       <c r="A144" s="4"/>
       <c r="B144" s="4"/>
       <c r="C144" s="4"/>
@@ -7051,7 +7072,7 @@
       <c r="AD144" s="3"/>
       <c r="AE144" s="47"/>
     </row>
-    <row r="145" spans="1:31" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:31" s="2" customFormat="1" ht="26.25" customHeight="1">
       <c r="A145" s="4"/>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
@@ -7078,7 +7099,7 @@
       <c r="AD145" s="3"/>
       <c r="AE145" s="47"/>
     </row>
-    <row r="146" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:31" s="2" customFormat="1">
       <c r="A146" s="4"/>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
@@ -7104,7 +7125,7 @@
       <c r="AD146" s="3"/>
       <c r="AE146" s="47"/>
     </row>
-    <row r="147" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:31" s="2" customFormat="1">
       <c r="A147" s="4"/>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
@@ -7129,7 +7150,7 @@
       <c r="AD147" s="3"/>
       <c r="AE147" s="47"/>
     </row>
-    <row r="148" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:31" s="2" customFormat="1">
       <c r="A148" s="4"/>
       <c r="B148" s="4"/>
       <c r="C148" s="4"/>
@@ -7156,7 +7177,7 @@
       <c r="AD148" s="3"/>
       <c r="AE148" s="47"/>
     </row>
-    <row r="149" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:31" s="2" customFormat="1">
       <c r="A149" s="4"/>
       <c r="B149" s="4"/>
       <c r="C149" s="4"/>
@@ -7184,7 +7205,7 @@
       <c r="AD149" s="3"/>
       <c r="AE149" s="47"/>
     </row>
-    <row r="150" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:31" s="2" customFormat="1">
       <c r="I150" s="3"/>
       <c r="U150" s="36"/>
       <c r="V150" s="36"/>
@@ -7194,7 +7215,7 @@
       <c r="AD150" s="3"/>
       <c r="AE150" s="47"/>
     </row>
-    <row r="151" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:31" s="2" customFormat="1">
       <c r="J151" s="3"/>
       <c r="U151" s="36"/>
       <c r="V151" s="36"/>
@@ -7204,7 +7225,7 @@
       <c r="AD151" s="3"/>
       <c r="AE151" s="47"/>
     </row>
-    <row r="152" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:31" s="2" customFormat="1">
       <c r="U152" s="36"/>
       <c r="V152" s="36"/>
       <c r="W152" s="36"/>
@@ -7213,7 +7234,7 @@
       <c r="AD152" s="3"/>
       <c r="AE152" s="47"/>
     </row>
-    <row r="153" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:31" s="2" customFormat="1">
       <c r="U153" s="36"/>
       <c r="V153" s="36"/>
       <c r="W153" s="36"/>
@@ -7222,7 +7243,7 @@
       <c r="AD153" s="3"/>
       <c r="AE153" s="47"/>
     </row>
-    <row r="154" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:31" s="2" customFormat="1">
       <c r="U154" s="36"/>
       <c r="V154" s="36"/>
       <c r="W154" s="36"/>
@@ -7231,7 +7252,7 @@
       <c r="AD154" s="3"/>
       <c r="AE154" s="47"/>
     </row>
-    <row r="155" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:31" s="2" customFormat="1">
       <c r="U155" s="36"/>
       <c r="V155" s="36"/>
       <c r="W155" s="36"/>
@@ -7240,7 +7261,7 @@
       <c r="AD155" s="3"/>
       <c r="AE155" s="47"/>
     </row>
-    <row r="156" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:31" s="2" customFormat="1">
       <c r="U156" s="36"/>
       <c r="V156" s="36"/>
       <c r="W156" s="36"/>
@@ -7249,7 +7270,7 @@
       <c r="AD156" s="3"/>
       <c r="AE156" s="47"/>
     </row>
-    <row r="157" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:31" s="2" customFormat="1">
       <c r="U157" s="36"/>
       <c r="V157" s="36"/>
       <c r="W157" s="36"/>
@@ -7258,7 +7279,7 @@
       <c r="AD157" s="3"/>
       <c r="AE157" s="47"/>
     </row>
-    <row r="158" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:31" s="2" customFormat="1">
       <c r="U158" s="36"/>
       <c r="V158" s="36"/>
       <c r="W158" s="36"/>
@@ -7267,7 +7288,7 @@
       <c r="AD158" s="3"/>
       <c r="AE158" s="47"/>
     </row>
-    <row r="159" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:31" s="2" customFormat="1">
       <c r="U159" s="36"/>
       <c r="V159" s="36"/>
       <c r="W159" s="36"/>
@@ -7276,7 +7297,7 @@
       <c r="AD159" s="3"/>
       <c r="AE159" s="47"/>
     </row>
-    <row r="160" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:31" s="2" customFormat="1">
       <c r="U160" s="36"/>
       <c r="V160" s="36"/>
       <c r="W160" s="36"/>
@@ -7285,7 +7306,7 @@
       <c r="AD160" s="3"/>
       <c r="AE160" s="47"/>
     </row>
-    <row r="161" spans="21:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="21:31" s="2" customFormat="1">
       <c r="U161" s="36"/>
       <c r="V161" s="36"/>
       <c r="W161" s="36"/>
@@ -7294,7 +7315,7 @@
       <c r="AD161" s="3"/>
       <c r="AE161" s="47"/>
     </row>
-    <row r="162" spans="21:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="21:31" s="2" customFormat="1">
       <c r="U162" s="36"/>
       <c r="V162" s="36"/>
       <c r="W162" s="36"/>
@@ -7303,7 +7324,7 @@
       <c r="AD162" s="3"/>
       <c r="AE162" s="47"/>
     </row>
-    <row r="163" spans="21:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="21:31" s="2" customFormat="1">
       <c r="U163" s="36"/>
       <c r="V163" s="36"/>
       <c r="W163" s="36"/>
@@ -7312,7 +7333,7 @@
       <c r="AD163" s="3"/>
       <c r="AE163" s="47"/>
     </row>
-    <row r="164" spans="21:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="21:31" s="2" customFormat="1">
       <c r="U164" s="36"/>
       <c r="V164" s="36"/>
       <c r="W164" s="36"/>
@@ -7321,7 +7342,7 @@
       <c r="AD164" s="3"/>
       <c r="AE164" s="47"/>
     </row>
-    <row r="165" spans="21:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="21:31" s="2" customFormat="1">
       <c r="U165" s="36"/>
       <c r="V165" s="36"/>
       <c r="W165" s="36"/>
@@ -7330,7 +7351,7 @@
       <c r="AD165" s="3"/>
       <c r="AE165" s="47"/>
     </row>
-    <row r="166" spans="21:31" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="21:31" s="2" customFormat="1">
       <c r="U166" s="36"/>
       <c r="V166" s="36"/>
       <c r="W166" s="36"/>
@@ -7347,28 +7368,33 @@
     <mergeCell ref="V2:W2"/>
   </mergeCells>
   <pageMargins left="0.35433070866141736" right="0.35433070866141736" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="8" scale="80" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="8" scale="80" orientation="landscape"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Blad1"/>
+  <sheetPr codeName="Blad1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="49" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" customWidth="1"/>
-    <col min="3" max="3" width="78.140625" style="75" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" customWidth="1"/>
+    <col min="3" max="3" width="78.1640625" style="75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="17" t="s">
         <v>172</v>
       </c>
@@ -7379,7 +7405,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="36">
       <c r="A3" s="73" t="s">
         <v>175</v>
       </c>
@@ -7390,7 +7416,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="36">
       <c r="A5" s="73" t="s">
         <v>187</v>
       </c>
@@ -7401,10 +7427,15 @@
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="I9" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>